<commit_message>
update CA US SUM USCA file
</commit_message>
<xml_diff>
--- a/ComplexNetwork1/src/result/CA.xlsx
+++ b/ComplexNetwork1/src/result/CA.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="basic_information" sheetId="4" r:id="rId1"/>
+    <sheet name="connected component" sheetId="5" r:id="rId1"/>
     <sheet name="degree" sheetId="2" r:id="rId2"/>
     <sheet name="clossness" sheetId="3" r:id="rId3"/>
     <sheet name="betweenness" sheetId="1" r:id="rId4"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="177">
   <si>
     <t>[CAYWK]</t>
   </si>
@@ -540,10 +540,19 @@
     <t>[CAYZP]</t>
   </si>
   <si>
-    <t>CA_vertice</t>
-  </si>
-  <si>
-    <t>CA_edge</t>
+    <t>total vertices is: 172</t>
+  </si>
+  <si>
+    <t>Component 1: [CAYGL, CAYGW, CAYPX, CAYUL, CAYUY, CAYVP, CAYQB, CAYWK, CAYZV, CAYEG, CAYVR, CAYOW, CAYYC, CAYWG, CAYYZ, CAYBC, CAYYY, CAYBG, CAYHZ, CAYYT, CAYFC, CAYQM, CAYSJ, CAYYG, CAYTZ, CAYVO, CAZBF, CAYMT, CAYKQ, CAYMO, CAZEM, CAYNC, CAYTS, CAYFA, CAZKE, CAYAT, CAYPO, CAYQT, CAYSB, CAYYU, CAYAM, CAYYB, CAYAG, CAYHD, CAYXL, CAYFH, CAYWP, CAYPL, CAYLH, CAYRL, CAYAC, CAZRJ, CAYAX, CAYTL, CAYER, CAYPM, CAZSJ, CAZPB, CAYVZ, CAYQK, CAYVB, CAYGR, CAYGP, CAYHU, CAYQG, CAYHM, CAYDF, CAYYR, CAYQX, CAYAY, CAYJT, CAYBX, CAYIF, CAYHR, CAYNA, CAYDP, CAZUM, CAYQY, CAYCL, CAYLW, CAYYJ, CAYMM, CAYQR, CAYXE, CAYGK, CAYXU, CAYZR, CAYQF, CAYPY, CAYSM, CAYZF, CAYHY, CAYXY, CAYCB, CAYCO, CAYYH, CAYRT, CAYVQ, CAYHK, CAYFS, CAYFJ, CAYRA, CAYSG, CAYWJ, CAZFN, CAYEV, CAYGH, CAYHI, CAYPC, CAYSY, CAYUB, CAZFM, CAYBK, CAYCS, CAYXN, CAYFB, CAYEK, CAYYQ, CAYUT, CAYZS, CAYTH, CAYFO, CAYQD, CAYGX, CAYTE, CAYCY, CAYGT, CAYUX, CAYXP, CAYLC, CAYVM, CAYIO, CAYXC, CAYXS, CAYYE, CAYXJ, CAYKA, CAYXT, CAYYD, CAYDQ, CAYSK, CAYQQ, CAYLL, CAYCD, CAYCG, CAYQU, CAYQL, CAYXH, CAYBR, CAYXX, CAYKF, CAYBL, CAYPW, CAYWL, CAYZT, CAZMT, CAYQZ, CAYPR, CAYYF, CAYZP, CAYOJ, CAYOP, CAYKL, CAYGV, CAYPN, CAYPH, CAYKG, CAYTQ]</t>
+  </si>
+  <si>
+    <t>Component 2: [CAYIK, CAYZG]</t>
+  </si>
+  <si>
+    <t>Component 3: [CAYGZ, CAYRB]</t>
+  </si>
+  <si>
+    <t>total edges is: 370</t>
   </si>
 </sst>
 </file>
@@ -860,33 +869,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C2D2F9-3AC8-4F59-A384-CE65E5134CD5}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52AAC221-1017-4E5D-95BC-E2C148338964}">
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>172</v>
       </c>
-      <c r="B1">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>173</v>
       </c>
-      <c r="B2">
-        <v>1039</v>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data of pageRank
</commit_message>
<xml_diff>
--- a/ComplexNetwork1/src/result/CA.xlsx
+++ b/ComplexNetwork1/src/result/CA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="connected component" sheetId="5" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="betweenness" sheetId="1" r:id="rId4"/>
     <sheet name="density" sheetId="6" r:id="rId5"/>
     <sheet name="clustering coefficient" sheetId="7" r:id="rId6"/>
+    <sheet name="pageRank" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="523">
   <si>
     <t>[CAYWK]</t>
   </si>
@@ -1077,6 +1078,522 @@
   </si>
   <si>
     <t>CAYZP: 0.0</t>
+  </si>
+  <si>
+    <t>CAYWK: 0.6085755960976994</t>
+  </si>
+  <si>
+    <t>CAYWJ: 0.24109125671940038</t>
+  </si>
+  <si>
+    <t>CAYWG: 0.9800828853228987</t>
+  </si>
+  <si>
+    <t>CAYFS: 0.1513954755488643</t>
+  </si>
+  <si>
+    <t>CAYFO: 0.2395943184668877</t>
+  </si>
+  <si>
+    <t>CAYGK: 0.1348166008352925</t>
+  </si>
+  <si>
+    <t>CAYOP: 0.20980416011955139</t>
+  </si>
+  <si>
+    <t>CAYGH: 0.25304459749626695</t>
+  </si>
+  <si>
+    <t>CAYOJ: 0.20980416898862125</t>
+  </si>
+  <si>
+    <t>CAYWP: 0.30664273353511834</t>
+  </si>
+  <si>
+    <t>CAYWL: 0.2215440640249542</t>
+  </si>
+  <si>
+    <t>CAYXL: 0.879826234881961</t>
+  </si>
+  <si>
+    <t>CAYGZ: 0.33333336828892207</t>
+  </si>
+  <si>
+    <t>CAYPC: 0.18115288701701868</t>
+  </si>
+  <si>
+    <t>CAYXJ: 0.32443794629794653</t>
+  </si>
+  <si>
+    <t>CAYGX: 0.1836889702227043</t>
+  </si>
+  <si>
+    <t>CAYGW: 0.4327445857283516</t>
+  </si>
+  <si>
+    <t>CAYXH: 0.13998273091512198</t>
+  </si>
+  <si>
+    <t>CAYGV: 0.221346822657079</t>
+  </si>
+  <si>
+    <t>CAYGT: 0.33886320849820173</t>
+  </si>
+  <si>
+    <t>CAYXE: 0.29128398340571926</t>
+  </si>
+  <si>
+    <t>CAYXC: 0.2218136070089129</t>
+  </si>
+  <si>
+    <t>CAYGR: 0.2511564793942326</t>
+  </si>
+  <si>
+    <t>CAYGP: 0.19452655083024212</t>
+  </si>
+  <si>
+    <t>CAYOW: 0.7105370542429214</t>
+  </si>
+  <si>
+    <t>CAYGL: 0.24940199844009867</t>
+  </si>
+  <si>
+    <t>CAYHK: 0.277092121785632</t>
+  </si>
+  <si>
+    <t>CAYPR: 0.14400363385408516</t>
+  </si>
+  <si>
+    <t>CAYXY: 0.3095818510469943</t>
+  </si>
+  <si>
+    <t>CAYHI: 0.34046636521171436</t>
+  </si>
+  <si>
+    <t>CAYXX: 0.17635543188865593</t>
+  </si>
+  <si>
+    <t>CAYPO: 0.23326652991324054</t>
+  </si>
+  <si>
+    <t>CAYPN: 0.22134681682250662</t>
+  </si>
+  <si>
+    <t>CAYXU: 0.24406604444276989</t>
+  </si>
+  <si>
+    <t>CAYPM: 0.3143536336219239</t>
+  </si>
+  <si>
+    <t>CAYXT: 0.2443317318632756</t>
+  </si>
+  <si>
+    <t>CAYHD: 0.3000195949749606</t>
+  </si>
+  <si>
+    <t>CAYPL: 0.2146592467318236</t>
+  </si>
+  <si>
+    <t>CAYXS: 0.4950554653262319</t>
+  </si>
+  <si>
+    <t>CAZRJ: 0.23280492060598407</t>
+  </si>
+  <si>
+    <t>CAYPH: 0.27124507758043803</t>
+  </si>
+  <si>
+    <t>CAYXP: 0.30590729149023016</t>
+  </si>
+  <si>
+    <t>CAYXN: 0.2626484599232371</t>
+  </si>
+  <si>
+    <t>CAYUB: 0.18115288701701868</t>
+  </si>
+  <si>
+    <t>CAYDQ: 0.20476516465056047</t>
+  </si>
+  <si>
+    <t>CAYDP: 0.1474129387184554</t>
+  </si>
+  <si>
+    <t>CAYLW: 0.4863502573676459</t>
+  </si>
+  <si>
+    <t>CAZFN: 0.256273660487246</t>
+  </si>
+  <si>
+    <t>CAZFM: 0.18115288701701868</t>
+  </si>
+  <si>
+    <t>CAYTZ: 0.43109186422645307</t>
+  </si>
+  <si>
+    <t>CAYUY: 0.2390390728280849</t>
+  </si>
+  <si>
+    <t>CAYUX: 0.24002808095617234</t>
+  </si>
+  <si>
+    <t>CAYEG: 1.1431420305967814</t>
+  </si>
+  <si>
+    <t>CAYMO: 0.32154885154415197</t>
+  </si>
+  <si>
+    <t>CAYMM: 0.376522265245143</t>
+  </si>
+  <si>
+    <t>CAYUT: 0.26314611517523223</t>
+  </si>
+  <si>
+    <t>CAYUL: 1.2690404400947906</t>
+  </si>
+  <si>
+    <t>CAYNA: 0.24119960707160387</t>
+  </si>
+  <si>
+    <t>CAZPB: 0.15132319703478106</t>
+  </si>
+  <si>
+    <t>CAYEV: 0.8115288701701867</t>
+  </si>
+  <si>
+    <t>CAYER: 0.2837310000870396</t>
+  </si>
+  <si>
+    <t>CAYVB: 0.33677725958358407</t>
+  </si>
+  <si>
+    <t>CAYMT: 0.2066416958928582</t>
+  </si>
+  <si>
+    <t>CAYEK: 0.2569086486499763</t>
+  </si>
+  <si>
+    <t>CAYFJ: 0.1513954755488643</t>
+  </si>
+  <si>
+    <t>CAYVZ: 0.2578721481347357</t>
+  </si>
+  <si>
+    <t>CAYFH: 0.23151200016385393</t>
+  </si>
+  <si>
+    <t>CAYFC: 0.23796120802036166</t>
+  </si>
+  <si>
+    <t>CAYVR: 1.9487323563951993</t>
+  </si>
+  <si>
+    <t>CAYFB: 0.783771415370468</t>
+  </si>
+  <si>
+    <t>CAYVQ: 0.41080977416713327</t>
+  </si>
+  <si>
+    <t>CAYFA: 0.29250298169761113</t>
+  </si>
+  <si>
+    <t>CAYVP: 0.6401097420062235</t>
+  </si>
+  <si>
+    <t>CAYVO: 0.3107755334439678</t>
+  </si>
+  <si>
+    <t>CAYVM: 0.20706755202158056</t>
+  </si>
+  <si>
+    <t>CAYNC: 0.21240573449222372</t>
+  </si>
+  <si>
+    <t>CAYSG: 0.1513954755488643</t>
+  </si>
+  <si>
+    <t>CAYBR: 0.13998273091512198</t>
+  </si>
+  <si>
+    <t>CAYSB: 0.36992592686258585</t>
+  </si>
+  <si>
+    <t>CAYBL: 0.19447827622567634</t>
+  </si>
+  <si>
+    <t>CAYJT: 0.18452144768075524</t>
+  </si>
+  <si>
+    <t>CAYBK: 0.32918239628103474</t>
+  </si>
+  <si>
+    <t>CAYBG: 0.30105084522415415</t>
+  </si>
+  <si>
+    <t>CAYCG: 0.1839863647692071</t>
+  </si>
+  <si>
+    <t>CAYKL: 0.2745359735825577</t>
+  </si>
+  <si>
+    <t>CAYCD: 0.1839863647692071</t>
+  </si>
+  <si>
+    <t>CAYCB: 0.34881037605590104</t>
+  </si>
+  <si>
+    <t>CAYKG: 0.15600961944172737</t>
+  </si>
+  <si>
+    <t>CAYKF: 0.13998273091512198</t>
+  </si>
+  <si>
+    <t>CAYSM: 0.31401067801155136</t>
+  </si>
+  <si>
+    <t>CAZUM: 0.18614047665194536</t>
+  </si>
+  <si>
+    <t>CAYSK: 0.1865951989504465</t>
+  </si>
+  <si>
+    <t>CAYSJ: 0.20480281215569202</t>
+  </si>
+  <si>
+    <t>CAYKA: 0.22730372932996404</t>
+  </si>
+  <si>
+    <t>CAYBX: 0.3010499025332129</t>
+  </si>
+  <si>
+    <t>CAYTH: 0.40783417195730176</t>
+  </si>
+  <si>
+    <t>CAYTE: 0.22140304072034572</t>
+  </si>
+  <si>
+    <t>CAYCS: 0.26314613345597065</t>
+  </si>
+  <si>
+    <t>CAYCO: 0.29187945365274837</t>
+  </si>
+  <si>
+    <t>CAYCL: 0.174547275866722</t>
+  </si>
+  <si>
+    <t>CAZEM: 0.32115924140635344</t>
+  </si>
+  <si>
+    <t>CAZMT: 0.14400363385408516</t>
+  </si>
+  <si>
+    <t>CAYSY: 0.260595038899752</t>
+  </si>
+  <si>
+    <t>CAYKQ: 0.4141441286039471</t>
+  </si>
+  <si>
+    <t>CAYDF: 0.3220642776296798</t>
+  </si>
+  <si>
+    <t>CAYLL: 0.13998273091512198</t>
+  </si>
+  <si>
+    <t>CAYTS: 0.4002649327605129</t>
+  </si>
+  <si>
+    <t>CAYTQ: 0.15600960242554457</t>
+  </si>
+  <si>
+    <t>CAYLH: 0.2525791809442863</t>
+  </si>
+  <si>
+    <t>CAYTL: 0.28373100413219743</t>
+  </si>
+  <si>
+    <t>CAYLC: 0.16095999897325863</t>
+  </si>
+  <si>
+    <t>CAYCY: 0.25485339806492513</t>
+  </si>
+  <si>
+    <t>CAYQD: 0.2395943111983114</t>
+  </si>
+  <si>
+    <t>CAYHZ: 0.7675658128549724</t>
+  </si>
+  <si>
+    <t>CAYQB: 0.7184672215063099</t>
+  </si>
+  <si>
+    <t>CAYHY: 0.24272005691868254</t>
+  </si>
+  <si>
+    <t>CAYYJ: 0.2930029233420861</t>
+  </si>
+  <si>
+    <t>CAYYH: 0.27709213040136443</t>
+  </si>
+  <si>
+    <t>CAYYG: 0.20480281215569202</t>
+  </si>
+  <si>
+    <t>CAYYF: 0.14400363385408516</t>
+  </si>
+  <si>
+    <t>CAYHU: 0.27633162665192035</t>
+  </si>
+  <si>
+    <t>CAYYE: 0.2604064971190653</t>
+  </si>
+  <si>
+    <t>CAYYD: 0.24433172450489474</t>
+  </si>
+  <si>
+    <t>CAYYC: 1.8277819846912897</t>
+  </si>
+  <si>
+    <t>CAYHR: 0.27806906687794997</t>
+  </si>
+  <si>
+    <t>CAYYB: 0.17797462563592753</t>
+  </si>
+  <si>
+    <t>CAYPY: 0.19887946626395483</t>
+  </si>
+  <si>
+    <t>CAYPX: 0.2774939563017271</t>
+  </si>
+  <si>
+    <t>CAYPW: 0.14400363385408516</t>
+  </si>
+  <si>
+    <t>CAZBF: 0.1813152989154998</t>
+  </si>
+  <si>
+    <t>CAYHM: 0.25165529514783724</t>
+  </si>
+  <si>
+    <t>CAYQU: 0.17635543188865593</t>
+  </si>
+  <si>
+    <t>CAYQT: 0.8006008320816873</t>
+  </si>
+  <si>
+    <t>CAYIK: 0.33333336828892207</t>
+  </si>
+  <si>
+    <t>CAYAC: 0.23280492448915147</t>
+  </si>
+  <si>
+    <t>CAYYZ: 1.442402034604976</t>
+  </si>
+  <si>
+    <t>CAYQR: 0.29128398340571926</t>
+  </si>
+  <si>
+    <t>CAYQQ: 0.28842646242172776</t>
+  </si>
+  <si>
+    <t>CAYYY: 0.34339566367742336</t>
+  </si>
+  <si>
+    <t>CAYIF: 0.2675691554368246</t>
+  </si>
+  <si>
+    <t>CAYQM: 0.2820008951853523</t>
+  </si>
+  <si>
+    <t>CAYYU: 0.18980685106235584</t>
+  </si>
+  <si>
+    <t>CAYYT: 0.5069886275905724</t>
+  </si>
+  <si>
+    <t>CAYQL: 0.13998273091512198</t>
+  </si>
+  <si>
+    <t>CAZKE: 0.33564258761597165</t>
+  </si>
+  <si>
+    <t>CAYQK: 0.24745170879134812</t>
+  </si>
+  <si>
+    <t>CAYYR: 0.6095949263801407</t>
+  </si>
+  <si>
+    <t>CAYYQ: 0.2887305034297961</t>
+  </si>
+  <si>
+    <t>CAZSJ: 0.314353623468964</t>
+  </si>
+  <si>
+    <t>CAYQG: 0.21251988038596165</t>
+  </si>
+  <si>
+    <t>CAYQF: 0.2217375707667611</t>
+  </si>
+  <si>
+    <t>CAYAT: 0.3807615140378301</t>
+  </si>
+  <si>
+    <t>CAYRB: 0.33333335780224543</t>
+  </si>
+  <si>
+    <t>CAYRA: 0.1513954755488643</t>
+  </si>
+  <si>
+    <t>CAYZG: 0.33333335780224543</t>
+  </si>
+  <si>
+    <t>CAYZF: 1.2481758347581324</t>
+  </si>
+  <si>
+    <t>CAYAM: 0.2588044911214399</t>
+  </si>
+  <si>
+    <t>CAYQZ: 0.2215440562628191</t>
+  </si>
+  <si>
+    <t>CAYQY: 0.17063633876852458</t>
+  </si>
+  <si>
+    <t>CAYQX: 0.22266512546428752</t>
+  </si>
+  <si>
+    <t>CAYIO: 0.2682667809531727</t>
+  </si>
+  <si>
+    <t>CAYAG: 0.25217122405356807</t>
+  </si>
+  <si>
+    <t>CAYRT: 0.7086538498122924</t>
+  </si>
+  <si>
+    <t>CAYBC: 0.24888021063193808</t>
+  </si>
+  <si>
+    <t>CAYZV: 0.6267918413218422</t>
+  </si>
+  <si>
+    <t>CAYZT: 0.14400363385408516</t>
+  </si>
+  <si>
+    <t>CAYRL: 0.4101289084477824</t>
+  </si>
+  <si>
+    <t>CAYZS: 0.3453887430116991</t>
+  </si>
+  <si>
+    <t>CAYZR: 0.1348166008352925</t>
+  </si>
+  <si>
+    <t>CAYAY: 0.2570903721817179</t>
+  </si>
+  <si>
+    <t>CAYAX: 0.28373100894891057</t>
+  </si>
+  <si>
+    <t>CAYZP: 0.14400363385408516</t>
   </si>
 </sst>
 </file>
@@ -5694,8 +6211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F079C9-CD16-42EC-89E2-F8F8F9D8DC50}">
   <dimension ref="A1:A173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6571,4 +7088,892 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38614E5-E495-4BD6-86CD-437E1B55E538}">
+  <dimension ref="A1:A175"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>522</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change the format of data
</commit_message>
<xml_diff>
--- a/ComplexNetwork1/src/result/CA.xlsx
+++ b/ComplexNetwork1/src/result/CA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="connected component" sheetId="5" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="betweenness" sheetId="1" r:id="rId4"/>
     <sheet name="density" sheetId="6" r:id="rId5"/>
     <sheet name="clustering coefficient" sheetId="7" r:id="rId6"/>
+    <sheet name="pageRank" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="351">
   <si>
     <t>[CAYWK]</t>
   </si>
@@ -563,520 +564,520 @@
     <t>the average clustering coefficient is: 0.43987601150772704</t>
   </si>
   <si>
-    <t>CAYWK: 0.3090909090909091</t>
-  </si>
-  <si>
-    <t>CAYWJ: 0.0</t>
-  </si>
-  <si>
-    <t>CAYWG: 0.19883040935672514</t>
-  </si>
-  <si>
-    <t>CAYFS: 0.0</t>
-  </si>
-  <si>
-    <t>CAYFO: 1.0</t>
-  </si>
-  <si>
-    <t>CAYGK: 0.0</t>
-  </si>
-  <si>
-    <t>CAYOP: 1.0</t>
-  </si>
-  <si>
-    <t>CAYGH: 1.0</t>
-  </si>
-  <si>
-    <t>CAYOJ: 1.0</t>
-  </si>
-  <si>
-    <t>CAYWP: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>CAYWL: 1.0</t>
-  </si>
-  <si>
-    <t>CAYXL: 0.15151515151515152</t>
-  </si>
-  <si>
-    <t>CAYGZ: 0.0</t>
-  </si>
-  <si>
-    <t>CAYPC: 0.0</t>
-  </si>
-  <si>
-    <t>CAYXJ: 0.6</t>
-  </si>
-  <si>
-    <t>CAYGX: 1.0</t>
-  </si>
-  <si>
-    <t>CAYGW: 0.26666666666666666</t>
-  </si>
-  <si>
-    <t>CAYXH: 0.0</t>
-  </si>
-  <si>
-    <t>CAYGV: 1.0</t>
-  </si>
-  <si>
-    <t>CAYGT: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>CAYXE: 1.0</t>
-  </si>
-  <si>
-    <t>CAYXC: 1.0</t>
-  </si>
-  <si>
-    <t>CAYGR: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>CAYGP: 1.0</t>
-  </si>
-  <si>
-    <t>CAYOW: 0.34285714285714286</t>
-  </si>
-  <si>
-    <t>CAYGL: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>CAYHK: 1.0</t>
-  </si>
-  <si>
-    <t>CAYPR: 0.0</t>
-  </si>
-  <si>
-    <t>CAYXY: 0.8</t>
-  </si>
-  <si>
-    <t>CAYHI: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>CAYXX: 1.0</t>
-  </si>
-  <si>
-    <t>CAYPO: 0.0</t>
-  </si>
-  <si>
-    <t>CAYPN: 1.0</t>
-  </si>
-  <si>
-    <t>CAYXU: 1.0</t>
-  </si>
-  <si>
-    <t>CAYPM: 0.8333333333333334</t>
-  </si>
-  <si>
-    <t>CAYXT: 1.0</t>
-  </si>
-  <si>
-    <t>CAYHD: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>CAYPL: 1.0</t>
-  </si>
-  <si>
-    <t>CAYXS: 0.39285714285714285</t>
-  </si>
-  <si>
-    <t>CAZRJ: 1.0</t>
-  </si>
-  <si>
-    <t>CAYPH: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>CAYXP: 0.0</t>
-  </si>
-  <si>
-    <t>CAYXN: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>CAYUB: 0.0</t>
-  </si>
-  <si>
-    <t>CAYDQ: 0.0</t>
-  </si>
-  <si>
-    <t>CAYDP: 0.0</t>
-  </si>
-  <si>
-    <t>CAYLW: 0.5</t>
-  </si>
-  <si>
-    <t>CAZFN: 0.0</t>
-  </si>
-  <si>
-    <t>CAZFM: 0.0</t>
-  </si>
-  <si>
-    <t>CAYTZ: 0.2857142857142857</t>
-  </si>
-  <si>
-    <t>CAYUY: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>CAYUX: 1.0</t>
-  </si>
-  <si>
-    <t>CAYEG: 0.21645021645021645</t>
-  </si>
-  <si>
-    <t>CAYMO: 0.0</t>
-  </si>
-  <si>
-    <t>CAYMM: 0.4666666666666667</t>
-  </si>
-  <si>
-    <t>CAYUT: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>CAYUL: 0.15692307692307692</t>
-  </si>
-  <si>
-    <t>CAYNA: 0.0</t>
-  </si>
-  <si>
-    <t>CAZPB: 0.0</t>
-  </si>
-  <si>
-    <t>CAYEV: 0.09523809523809523</t>
-  </si>
-  <si>
-    <t>CAYER: 1.0</t>
-  </si>
-  <si>
-    <t>CAYVB: 0.4</t>
-  </si>
-  <si>
-    <t>CAYMT: 0.0</t>
-  </si>
-  <si>
-    <t>CAYEK: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>CAYFJ: 0.0</t>
-  </si>
-  <si>
-    <t>CAYVZ: 1.0</t>
-  </si>
-  <si>
-    <t>CAYFH: 0.0</t>
-  </si>
-  <si>
-    <t>CAYFC: 1.0</t>
-  </si>
-  <si>
-    <t>CAYVR: 0.11612903225806452</t>
-  </si>
-  <si>
-    <t>CAYFB: 0.027777777777777776</t>
-  </si>
-  <si>
-    <t>CAYVQ: 0.16666666666666666</t>
-  </si>
-  <si>
-    <t>CAYFA: 0.0</t>
-  </si>
-  <si>
-    <t>CAYVP: 0.10714285714285714</t>
-  </si>
-  <si>
-    <t>CAYVO: 0.16666666666666666</t>
-  </si>
-  <si>
-    <t>CAYVM: 0.0</t>
-  </si>
-  <si>
-    <t>CAYNC: 0.0</t>
-  </si>
-  <si>
-    <t>CAYSG: 0.0</t>
-  </si>
-  <si>
-    <t>CAYBR: 0.0</t>
-  </si>
-  <si>
-    <t>CAYSB: 0.6</t>
-  </si>
-  <si>
-    <t>CAYBL: 1.0</t>
-  </si>
-  <si>
-    <t>CAYJT: 1.0</t>
-  </si>
-  <si>
-    <t>CAYBK: 0.5</t>
-  </si>
-  <si>
-    <t>CAYBG: 0.8</t>
-  </si>
-  <si>
-    <t>CAYCG: 1.0</t>
-  </si>
-  <si>
-    <t>CAYKL: 0.5</t>
-  </si>
-  <si>
-    <t>CAYCD: 1.0</t>
-  </si>
-  <si>
-    <t>CAYCB: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>CAYKG: 0.0</t>
-  </si>
-  <si>
-    <t>CAYKF: 0.0</t>
-  </si>
-  <si>
-    <t>CAYSM: 0.5</t>
-  </si>
-  <si>
-    <t>CAZUM: 1.0</t>
-  </si>
-  <si>
-    <t>CAYSK: 0.0</t>
-  </si>
-  <si>
-    <t>CAYSJ: 1.0</t>
-  </si>
-  <si>
-    <t>CAYKA: 1.0</t>
-  </si>
-  <si>
-    <t>CAYBX: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>CAYTH: 0.4666666666666667</t>
-  </si>
-  <si>
-    <t>CAYTE: 0.0</t>
-  </si>
-  <si>
-    <t>CAYCS: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>CAYCO: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>CAYCL: 0.0</t>
-  </si>
-  <si>
-    <t>CAZEM: 0.0</t>
-  </si>
-  <si>
-    <t>CAZMT: 0.0</t>
-  </si>
-  <si>
-    <t>CAYSY: 1.0</t>
-  </si>
-  <si>
-    <t>CAYKQ: 0.0</t>
-  </si>
-  <si>
-    <t>CAYDF: 0.6</t>
-  </si>
-  <si>
-    <t>CAYLL: 0.0</t>
-  </si>
-  <si>
-    <t>CAYTS: 0.4</t>
-  </si>
-  <si>
-    <t>CAYTQ: 0.0</t>
-  </si>
-  <si>
-    <t>CAYLH: 0.0</t>
-  </si>
-  <si>
-    <t>CAYTL: 1.0</t>
-  </si>
-  <si>
-    <t>CAYLC: 0.0</t>
-  </si>
-  <si>
-    <t>CAYCY: 0.0</t>
-  </si>
-  <si>
-    <t>CAYQD: 1.0</t>
-  </si>
-  <si>
-    <t>CAYHZ: 0.26666666666666666</t>
-  </si>
-  <si>
-    <t>CAYQB: 0.27472527472527475</t>
-  </si>
-  <si>
-    <t>CAYHY: 1.0</t>
-  </si>
-  <si>
-    <t>CAYYJ: 1.0</t>
-  </si>
-  <si>
-    <t>CAYYH: 1.0</t>
-  </si>
-  <si>
-    <t>CAYYG: 1.0</t>
-  </si>
-  <si>
-    <t>CAYYF: 0.0</t>
-  </si>
-  <si>
-    <t>CAYHU: 0.5</t>
-  </si>
-  <si>
-    <t>CAYYE: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>CAYYD: 1.0</t>
-  </si>
-  <si>
-    <t>CAYYC: 0.1310483870967742</t>
-  </si>
-  <si>
-    <t>CAYHR: 0.0</t>
-  </si>
-  <si>
-    <t>CAYYB: 1.0</t>
-  </si>
-  <si>
-    <t>CAYPY: 0.0</t>
-  </si>
-  <si>
-    <t>CAYPX: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>CAYPW: 0.0</t>
-  </si>
-  <si>
-    <t>CAZBF: 0.0</t>
-  </si>
-  <si>
-    <t>CAYHM: 0.5</t>
-  </si>
-  <si>
-    <t>CAYQU: 1.0</t>
-  </si>
-  <si>
-    <t>CAYQT: 0.16666666666666666</t>
-  </si>
-  <si>
-    <t>CAYIK: 0.0</t>
-  </si>
-  <si>
-    <t>CAYAC: 1.0</t>
-  </si>
-  <si>
-    <t>CAYYZ: 0.16009852216748768</t>
-  </si>
-  <si>
-    <t>CAYQR: 1.0</t>
-  </si>
-  <si>
-    <t>CAYQQ: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>CAYYY: 0.7333333333333333</t>
-  </si>
-  <si>
-    <t>CAYIF: 0.0</t>
-  </si>
-  <si>
-    <t>CAYQM: 0.7</t>
-  </si>
-  <si>
-    <t>CAYYU: 1.0</t>
-  </si>
-  <si>
-    <t>CAYYT: 0.3888888888888889</t>
-  </si>
-  <si>
-    <t>CAYQL: 0.0</t>
-  </si>
-  <si>
-    <t>CAZKE: 0.0</t>
-  </si>
-  <si>
-    <t>CAYQK: 0.0</t>
-  </si>
-  <si>
-    <t>CAYYR: 0.2222222222222222</t>
-  </si>
-  <si>
-    <t>CAYYQ: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>CAZSJ: 0.8333333333333334</t>
-  </si>
-  <si>
-    <t>CAYQG: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>CAYQF: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>CAYAT: 0.0</t>
-  </si>
-  <si>
-    <t>CAYRB: 0.0</t>
-  </si>
-  <si>
-    <t>CAYRA: 0.0</t>
-  </si>
-  <si>
-    <t>CAYZG: 0.0</t>
-  </si>
-  <si>
-    <t>CAYZF: 0.08823529411764706</t>
-  </si>
-  <si>
-    <t>CAYAM: 0.8333333333333334</t>
-  </si>
-  <si>
-    <t>CAYQZ: 1.0</t>
-  </si>
-  <si>
-    <t>CAYQY: 1.0</t>
-  </si>
-  <si>
-    <t>CAYQX: 1.0</t>
-  </si>
-  <si>
-    <t>CAYIO: 0.0</t>
-  </si>
-  <si>
-    <t>CAYAG: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>CAYRT: 0.18181818181818182</t>
-  </si>
-  <si>
-    <t>CAYBC: 1.0</t>
-  </si>
-  <si>
-    <t>CAYZV: 0.3111111111111111</t>
-  </si>
-  <si>
-    <t>CAYZT: 0.0</t>
-  </si>
-  <si>
-    <t>CAYRL: 0.4</t>
-  </si>
-  <si>
-    <t>CAYZS: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>CAYZR: 0.0</t>
-  </si>
-  <si>
-    <t>CAYAY: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>CAYAX: 1.0</t>
-  </si>
-  <si>
-    <t>CAYZP: 0.0</t>
+    <t>CAYWK</t>
+  </si>
+  <si>
+    <t>CAYWJ</t>
+  </si>
+  <si>
+    <t>CAYWG</t>
+  </si>
+  <si>
+    <t>CAYFS</t>
+  </si>
+  <si>
+    <t>CAYFO</t>
+  </si>
+  <si>
+    <t>CAYGK</t>
+  </si>
+  <si>
+    <t>CAYOP</t>
+  </si>
+  <si>
+    <t>CAYGH</t>
+  </si>
+  <si>
+    <t>CAYOJ</t>
+  </si>
+  <si>
+    <t>CAYWP</t>
+  </si>
+  <si>
+    <t>CAYWL</t>
+  </si>
+  <si>
+    <t>CAYXL</t>
+  </si>
+  <si>
+    <t>CAYGZ</t>
+  </si>
+  <si>
+    <t>CAYPC</t>
+  </si>
+  <si>
+    <t>CAYXJ</t>
+  </si>
+  <si>
+    <t>CAYGX</t>
+  </si>
+  <si>
+    <t>CAYGW</t>
+  </si>
+  <si>
+    <t>CAYXH</t>
+  </si>
+  <si>
+    <t>CAYGV</t>
+  </si>
+  <si>
+    <t>CAYGT</t>
+  </si>
+  <si>
+    <t>CAYXE</t>
+  </si>
+  <si>
+    <t>CAYXC</t>
+  </si>
+  <si>
+    <t>CAYGR</t>
+  </si>
+  <si>
+    <t>CAYGP</t>
+  </si>
+  <si>
+    <t>CAYOW</t>
+  </si>
+  <si>
+    <t>CAYGL</t>
+  </si>
+  <si>
+    <t>CAYHK</t>
+  </si>
+  <si>
+    <t>CAYPR</t>
+  </si>
+  <si>
+    <t>CAYXY</t>
+  </si>
+  <si>
+    <t>CAYHI</t>
+  </si>
+  <si>
+    <t>CAYXX</t>
+  </si>
+  <si>
+    <t>CAYPO</t>
+  </si>
+  <si>
+    <t>CAYPN</t>
+  </si>
+  <si>
+    <t>CAYXU</t>
+  </si>
+  <si>
+    <t>CAYPM</t>
+  </si>
+  <si>
+    <t>CAYXT</t>
+  </si>
+  <si>
+    <t>CAYHD</t>
+  </si>
+  <si>
+    <t>CAYPL</t>
+  </si>
+  <si>
+    <t>CAYXS</t>
+  </si>
+  <si>
+    <t>CAZRJ</t>
+  </si>
+  <si>
+    <t>CAYPH</t>
+  </si>
+  <si>
+    <t>CAYXP</t>
+  </si>
+  <si>
+    <t>CAYXN</t>
+  </si>
+  <si>
+    <t>CAYUB</t>
+  </si>
+  <si>
+    <t>CAYDQ</t>
+  </si>
+  <si>
+    <t>CAYDP</t>
+  </si>
+  <si>
+    <t>CAYLW</t>
+  </si>
+  <si>
+    <t>CAZFN</t>
+  </si>
+  <si>
+    <t>CAZFM</t>
+  </si>
+  <si>
+    <t>CAYTZ</t>
+  </si>
+  <si>
+    <t>CAYUY</t>
+  </si>
+  <si>
+    <t>CAYUX</t>
+  </si>
+  <si>
+    <t>CAYEG</t>
+  </si>
+  <si>
+    <t>CAYMO</t>
+  </si>
+  <si>
+    <t>CAYMM</t>
+  </si>
+  <si>
+    <t>CAYUT</t>
+  </si>
+  <si>
+    <t>CAYUL</t>
+  </si>
+  <si>
+    <t>CAYNA</t>
+  </si>
+  <si>
+    <t>CAZPB</t>
+  </si>
+  <si>
+    <t>CAYEV</t>
+  </si>
+  <si>
+    <t>CAYER</t>
+  </si>
+  <si>
+    <t>CAYVB</t>
+  </si>
+  <si>
+    <t>CAYMT</t>
+  </si>
+  <si>
+    <t>CAYEK</t>
+  </si>
+  <si>
+    <t>CAYFJ</t>
+  </si>
+  <si>
+    <t>CAYVZ</t>
+  </si>
+  <si>
+    <t>CAYFH</t>
+  </si>
+  <si>
+    <t>CAYFC</t>
+  </si>
+  <si>
+    <t>CAYVR</t>
+  </si>
+  <si>
+    <t>CAYFB</t>
+  </si>
+  <si>
+    <t>CAYVQ</t>
+  </si>
+  <si>
+    <t>CAYFA</t>
+  </si>
+  <si>
+    <t>CAYVP</t>
+  </si>
+  <si>
+    <t>CAYVO</t>
+  </si>
+  <si>
+    <t>CAYVM</t>
+  </si>
+  <si>
+    <t>CAYNC</t>
+  </si>
+  <si>
+    <t>CAYSG</t>
+  </si>
+  <si>
+    <t>CAYBR</t>
+  </si>
+  <si>
+    <t>CAYSB</t>
+  </si>
+  <si>
+    <t>CAYBL</t>
+  </si>
+  <si>
+    <t>CAYJT</t>
+  </si>
+  <si>
+    <t>CAYBK</t>
+  </si>
+  <si>
+    <t>CAYBG</t>
+  </si>
+  <si>
+    <t>CAYCG</t>
+  </si>
+  <si>
+    <t>CAYKL</t>
+  </si>
+  <si>
+    <t>CAYCD</t>
+  </si>
+  <si>
+    <t>CAYCB</t>
+  </si>
+  <si>
+    <t>CAYKG</t>
+  </si>
+  <si>
+    <t>CAYKF</t>
+  </si>
+  <si>
+    <t>CAYSM</t>
+  </si>
+  <si>
+    <t>CAZUM</t>
+  </si>
+  <si>
+    <t>CAYSK</t>
+  </si>
+  <si>
+    <t>CAYSJ</t>
+  </si>
+  <si>
+    <t>CAYKA</t>
+  </si>
+  <si>
+    <t>CAYBX</t>
+  </si>
+  <si>
+    <t>CAYTH</t>
+  </si>
+  <si>
+    <t>CAYTE</t>
+  </si>
+  <si>
+    <t>CAYCS</t>
+  </si>
+  <si>
+    <t>CAYCO</t>
+  </si>
+  <si>
+    <t>CAYCL</t>
+  </si>
+  <si>
+    <t>CAZEM</t>
+  </si>
+  <si>
+    <t>CAZMT</t>
+  </si>
+  <si>
+    <t>CAYSY</t>
+  </si>
+  <si>
+    <t>CAYKQ</t>
+  </si>
+  <si>
+    <t>CAYDF</t>
+  </si>
+  <si>
+    <t>CAYLL</t>
+  </si>
+  <si>
+    <t>CAYTS</t>
+  </si>
+  <si>
+    <t>CAYTQ</t>
+  </si>
+  <si>
+    <t>CAYLH</t>
+  </si>
+  <si>
+    <t>CAYTL</t>
+  </si>
+  <si>
+    <t>CAYLC</t>
+  </si>
+  <si>
+    <t>CAYCY</t>
+  </si>
+  <si>
+    <t>CAYQD</t>
+  </si>
+  <si>
+    <t>CAYHZ</t>
+  </si>
+  <si>
+    <t>CAYQB</t>
+  </si>
+  <si>
+    <t>CAYHY</t>
+  </si>
+  <si>
+    <t>CAYYJ</t>
+  </si>
+  <si>
+    <t>CAYYH</t>
+  </si>
+  <si>
+    <t>CAYYG</t>
+  </si>
+  <si>
+    <t>CAYYF</t>
+  </si>
+  <si>
+    <t>CAYHU</t>
+  </si>
+  <si>
+    <t>CAYYE</t>
+  </si>
+  <si>
+    <t>CAYYD</t>
+  </si>
+  <si>
+    <t>CAYYC</t>
+  </si>
+  <si>
+    <t>CAYHR</t>
+  </si>
+  <si>
+    <t>CAYYB</t>
+  </si>
+  <si>
+    <t>CAYPY</t>
+  </si>
+  <si>
+    <t>CAYPX</t>
+  </si>
+  <si>
+    <t>CAYPW</t>
+  </si>
+  <si>
+    <t>CAZBF</t>
+  </si>
+  <si>
+    <t>CAYHM</t>
+  </si>
+  <si>
+    <t>CAYQU</t>
+  </si>
+  <si>
+    <t>CAYQT</t>
+  </si>
+  <si>
+    <t>CAYIK</t>
+  </si>
+  <si>
+    <t>CAYAC</t>
+  </si>
+  <si>
+    <t>CAYYZ</t>
+  </si>
+  <si>
+    <t>CAYQR</t>
+  </si>
+  <si>
+    <t>CAYQQ</t>
+  </si>
+  <si>
+    <t>CAYYY</t>
+  </si>
+  <si>
+    <t>CAYIF</t>
+  </si>
+  <si>
+    <t>CAYQM</t>
+  </si>
+  <si>
+    <t>CAYYU</t>
+  </si>
+  <si>
+    <t>CAYYT</t>
+  </si>
+  <si>
+    <t>CAYQL</t>
+  </si>
+  <si>
+    <t>CAZKE</t>
+  </si>
+  <si>
+    <t>CAYQK</t>
+  </si>
+  <si>
+    <t>CAYYR</t>
+  </si>
+  <si>
+    <t>CAYYQ</t>
+  </si>
+  <si>
+    <t>CAZSJ</t>
+  </si>
+  <si>
+    <t>CAYQG</t>
+  </si>
+  <si>
+    <t>CAYQF</t>
+  </si>
+  <si>
+    <t>CAYAT</t>
+  </si>
+  <si>
+    <t>CAYRB</t>
+  </si>
+  <si>
+    <t>CAYRA</t>
+  </si>
+  <si>
+    <t>CAYZG</t>
+  </si>
+  <si>
+    <t>CAYZF</t>
+  </si>
+  <si>
+    <t>CAYAM</t>
+  </si>
+  <si>
+    <t>CAYQZ</t>
+  </si>
+  <si>
+    <t>CAYQY</t>
+  </si>
+  <si>
+    <t>CAYQX</t>
+  </si>
+  <si>
+    <t>CAYIO</t>
+  </si>
+  <si>
+    <t>CAYAG</t>
+  </si>
+  <si>
+    <t>CAYRT</t>
+  </si>
+  <si>
+    <t>CAYBC</t>
+  </si>
+  <si>
+    <t>CAYZV</t>
+  </si>
+  <si>
+    <t>CAYZT</t>
+  </si>
+  <si>
+    <t>CAYRL</t>
+  </si>
+  <si>
+    <t>CAYZS</t>
+  </si>
+  <si>
+    <t>CAYZR</t>
+  </si>
+  <si>
+    <t>CAYAY</t>
+  </si>
+  <si>
+    <t>CAYAX</t>
+  </si>
+  <si>
+    <t>CAYZP</t>
   </si>
 </sst>
 </file>
@@ -5692,880 +5693,2812 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F079C9-CD16-42EC-89E2-F8F8F9D8DC50}">
-  <dimension ref="A1:A173"/>
+  <dimension ref="A1:B175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="1" max="1" width="33.5546875" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4">
+        <v>0.30909090909090903</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6">
+        <v>0.198830409356725</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B15">
+        <v>0.15151515151515099</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>192</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>194</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>195</v>
+      </c>
+      <c r="B20">
+        <v>0.266666666666666</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>197</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>198</v>
+      </c>
+      <c r="B23">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>199</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>200</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>201</v>
+      </c>
+      <c r="B26">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>202</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>203</v>
+      </c>
+      <c r="B28">
+        <v>0.34285714285714203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>204</v>
+      </c>
+      <c r="B29">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>205</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>206</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>207</v>
+      </c>
+      <c r="B32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>208</v>
+      </c>
+      <c r="B33">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>209</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>210</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>211</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>212</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>213</v>
+      </c>
+      <c r="B38">
+        <v>0.83333333333333304</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>214</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>215</v>
+      </c>
+      <c r="B40">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>216</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>217</v>
+      </c>
+      <c r="B42">
+        <v>0.39285714285714202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>218</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>219</v>
+      </c>
+      <c r="B44">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>220</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>221</v>
+      </c>
+      <c r="B46">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>222</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>223</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>224</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>225</v>
+      </c>
+      <c r="B50">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>226</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>227</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>228</v>
+      </c>
+      <c r="B53">
+        <v>0.28571428571428498</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>229</v>
+      </c>
+      <c r="B54">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>230</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>231</v>
+      </c>
+      <c r="B56">
+        <v>0.216450216450216</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>232</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>233</v>
+      </c>
+      <c r="B58">
+        <v>0.46666666666666601</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>234</v>
+      </c>
+      <c r="B59">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>235</v>
+      </c>
+      <c r="B60">
+        <v>0.156923076923076</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>236</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>237</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>238</v>
+      </c>
+      <c r="B63">
+        <v>9.5238095238095205E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>239</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>240</v>
+      </c>
+      <c r="B65">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>241</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>242</v>
+      </c>
+      <c r="B67">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>243</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>244</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>245</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>246</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>247</v>
+      </c>
+      <c r="B72">
+        <v>0.11612903225806399</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>248</v>
+      </c>
+      <c r="B73">
+        <v>2.77777777777777E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>249</v>
+      </c>
+      <c r="B74">
+        <v>0.16666666666666599</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>250</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>251</v>
+      </c>
+      <c r="B76">
+        <v>0.107142857142857</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>252</v>
+      </c>
+      <c r="B77">
+        <v>0.16666666666666599</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>253</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>254</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>255</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>256</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>257</v>
+      </c>
+      <c r="B82">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>258</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>259</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>260</v>
+      </c>
+      <c r="B85">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>261</v>
+      </c>
+      <c r="B86">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>262</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>263</v>
+      </c>
+      <c r="B88">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>264</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>265</v>
+      </c>
+      <c r="B90">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>266</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>267</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>268</v>
+      </c>
+      <c r="B93">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>269</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>270</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>271</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>272</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>273</v>
+      </c>
+      <c r="B98">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>274</v>
+      </c>
+      <c r="B99">
+        <v>0.46666666666666601</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>275</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>276</v>
+      </c>
+      <c r="B101">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>277</v>
+      </c>
+      <c r="B102">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>278</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>279</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>280</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>281</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>282</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>283</v>
+      </c>
+      <c r="B108">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>284</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>285</v>
+      </c>
+      <c r="B110">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>286</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>287</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>288</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>289</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>290</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>291</v>
+      </c>
+      <c r="B116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>292</v>
+      </c>
+      <c r="B117">
+        <v>0.266666666666666</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>293</v>
+      </c>
+      <c r="B118">
+        <v>0.27472527472527403</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>294</v>
+      </c>
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>295</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>296</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>297</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>298</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>299</v>
+      </c>
+      <c r="B124">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>300</v>
+      </c>
+      <c r="B125">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>301</v>
+      </c>
+      <c r="B126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>302</v>
+      </c>
+      <c r="B127">
+        <v>0.13104838709677399</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>303</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>304</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>305</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>306</v>
+      </c>
+      <c r="B131">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>307</v>
+      </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>308</v>
+      </c>
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>309</v>
+      </c>
+      <c r="B134">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>310</v>
+      </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>311</v>
+      </c>
+      <c r="B136">
+        <v>0.16666666666666599</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>312</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>313</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>314</v>
+      </c>
+      <c r="B139">
+        <v>0.16009852216748699</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>315</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>316</v>
+      </c>
+      <c r="B141">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>317</v>
+      </c>
+      <c r="B142">
+        <v>0.73333333333333295</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>318</v>
+      </c>
+      <c r="B143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>319</v>
+      </c>
+      <c r="B144">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>320</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>321</v>
+      </c>
+      <c r="B146">
+        <v>0.38888888888888801</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>322</v>
+      </c>
+      <c r="B147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>323</v>
+      </c>
+      <c r="B148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>324</v>
+      </c>
+      <c r="B149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>325</v>
+      </c>
+      <c r="B150">
+        <v>0.22222222222222199</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>326</v>
+      </c>
+      <c r="B151">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>327</v>
+      </c>
+      <c r="B152">
+        <v>0.83333333333333304</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>328</v>
+      </c>
+      <c r="B153">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>329</v>
+      </c>
+      <c r="B154">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>330</v>
+      </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>331</v>
+      </c>
+      <c r="B156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>332</v>
+      </c>
+      <c r="B157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>333</v>
+      </c>
+      <c r="B158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>334</v>
+      </c>
+      <c r="B159">
+        <v>8.8235294117646995E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>335</v>
+      </c>
+      <c r="B160">
+        <v>0.83333333333333304</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>336</v>
+      </c>
+      <c r="B161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>337</v>
+      </c>
+      <c r="B162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>338</v>
+      </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>339</v>
+      </c>
+      <c r="B164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>340</v>
+      </c>
+      <c r="B165">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>341</v>
+      </c>
+      <c r="B166">
+        <v>0.18181818181818099</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>342</v>
+      </c>
+      <c r="B167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>343</v>
+      </c>
+      <c r="B168">
+        <v>0.31111111111111101</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>344</v>
+      </c>
+      <c r="B169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>345</v>
+      </c>
+      <c r="B170">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>346</v>
+      </c>
+      <c r="B171">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>347</v>
+      </c>
+      <c r="B172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>348</v>
+      </c>
+      <c r="B173">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>349</v>
+      </c>
+      <c r="B174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>350</v>
+      </c>
+      <c r="B175">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{316DB294-BC15-4EE8-975C-59A65540C50A}">
+  <dimension ref="A1:B175"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B4">
+        <v>0.60857559609769896</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B5">
+        <v>0.24109125671939999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B6">
+        <v>0.980082885322898</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B7">
+        <v>0.15139547554886401</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B8">
+        <v>0.239594318466887</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B9">
+        <v>0.13481660083529201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B10">
+        <v>0.209804160119551</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B11">
+        <v>0.25304459749626601</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B12">
+        <v>0.209804168988621</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B13">
+        <v>0.30664273353511801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B14">
+        <v>0.221544064024954</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B15">
+        <v>0.87982623488196099</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B16">
+        <v>0.33333336828892202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B17">
+        <v>0.18115288701701801</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B18">
+        <v>0.32443794629794598</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B19">
+        <v>0.183688970222704</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B20">
+        <v>0.43274458572835101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B21">
+        <v>0.13998273091512101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B22">
+        <v>0.221346822657079</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B23">
+        <v>0.33886320849820101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B24">
+        <v>0.29128398340571898</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B25">
+        <v>0.22181360700891201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B26">
+        <v>0.25115647939423202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B27">
+        <v>0.19452655083024201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="B28">
+        <v>0.71053705424292102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="B29">
+        <v>0.249401998440098</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="B30">
+        <v>0.27709212178563197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="B31">
+        <v>0.14400363385408499</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="B32">
+        <v>0.30958185104699398</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="B33">
+        <v>0.34046636521171397</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="B34">
+        <v>0.17635543188865499</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="B35">
+        <v>0.23326652991324001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="B36">
+        <v>0.22134681682250601</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="B37">
+        <v>0.244066044442769</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="B38">
+        <v>0.31435363362192298</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="B39">
+        <v>0.244331731863275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="B40">
+        <v>0.30001959497496</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="B41">
+        <v>0.21465924673182299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="B42">
+        <v>0.49505546532623101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="B43">
+        <v>0.23280492060598401</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="B44">
+        <v>0.27124507758043798</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="B45">
+        <v>0.30590729149022999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="B46">
+        <v>0.26264845992323699</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="B47">
+        <v>0.18115288701701801</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="B48">
+        <v>0.20476516465055999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="B49">
+        <v>0.14741293871845501</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="B50">
+        <v>0.48635025736764498</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="B51">
+        <v>0.25627366048724598</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="B52">
+        <v>0.18115288701701801</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="B53">
+        <v>0.43109186422645301</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="B54">
+        <v>0.23903907282808401</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="B55">
+        <v>0.24002808095617201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="B56">
+        <v>1.1431420305967801</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="B57">
+        <v>0.32154885154415103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="B58">
+        <v>0.37652226524514298</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="B59">
+        <v>0.26314611517523201</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="B60">
+        <v>1.2690404400947899</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="B61">
+        <v>0.24119960707160301</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="B62">
+        <v>0.151323197034781</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="B63">
+        <v>0.81152887017018605</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="B64">
+        <v>0.283731000087039</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="B65">
+        <v>0.33677725958358401</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="B66">
+        <v>0.206641695892858</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="B67">
+        <v>0.25690864864997598</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="B68">
+        <v>0.15139547554886401</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+      <c r="B69">
+        <v>0.25787214813473502</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="B70">
+        <v>0.23151200016385301</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="B71">
+        <v>0.237961208020361</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+      <c r="B72">
+        <v>1.9487323563951899</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+      <c r="B73">
+        <v>0.78377141537046802</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+      <c r="B74">
+        <v>0.41080977416713299</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+      <c r="B75">
+        <v>0.29250298169761102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+      <c r="B76">
+        <v>0.64010974200622295</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+      <c r="B77">
+        <v>0.31077553344396702</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="B78">
+        <v>0.20706755202158</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+      <c r="B79">
+        <v>0.212405734492223</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+      <c r="B80">
+        <v>0.15139547554886401</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+      <c r="B81">
+        <v>0.13998273091512101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+      <c r="B82">
+        <v>0.36992592686258502</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+      <c r="B83">
+        <v>0.19447827622567601</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+      <c r="B84">
+        <v>0.18452144768075501</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+      <c r="B85">
+        <v>0.32918239628103402</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="B86">
+        <v>0.30105084522415398</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+      <c r="B87">
+        <v>0.18398636476920699</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+      <c r="B88">
+        <v>0.27453597358255699</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+      <c r="B89">
+        <v>0.18398636476920699</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+      <c r="B90">
+        <v>0.34881037605590098</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+      <c r="B91">
+        <v>0.156009619441727</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+      <c r="B92">
+        <v>0.13998273091512101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+      <c r="B93">
+        <v>0.31401067801155103</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+      <c r="B94">
+        <v>0.186140476651945</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+      <c r="B95">
+        <v>0.18659519895044599</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+      <c r="B96">
+        <v>0.20480281215569199</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+      <c r="B97">
+        <v>0.22730372932996401</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+      <c r="B98">
+        <v>0.30104990253321201</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+      <c r="B99">
+        <v>0.40783417195730098</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+      <c r="B100">
+        <v>0.221403040720345</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="B101">
+        <v>0.26314613345596999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+      <c r="B102">
+        <v>0.29187945365274798</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+      <c r="B103">
+        <v>0.174547275866722</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+      <c r="B104">
+        <v>0.32115924140635299</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+      <c r="B105">
+        <v>0.14400363385408499</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+      <c r="B106">
+        <v>0.260595038899752</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+      <c r="B107">
+        <v>0.414144128603947</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+      <c r="B108">
+        <v>0.32206427762967899</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+      <c r="B109">
+        <v>0.13998273091512101</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+      <c r="B110">
+        <v>0.400264932760512</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+      <c r="B111">
+        <v>0.15600960242554399</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+      <c r="B112">
+        <v>0.252579180944286</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+      <c r="B113">
+        <v>0.28373100413219698</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+      <c r="B114">
+        <v>0.16095999897325799</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+      <c r="B115">
+        <v>0.25485339806492502</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+      <c r="B116">
+        <v>0.23959431119831101</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+      <c r="B117">
+        <v>0.76756581285497205</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+      <c r="B118">
+        <v>0.71846722150630904</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
+      <c r="B119">
+        <v>0.24272005691868201</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+      <c r="B120">
+        <v>0.293002923342086</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+      <c r="B121">
+        <v>0.27709213040136399</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
+      <c r="B122">
+        <v>0.20480281215569199</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
+      <c r="B123">
+        <v>0.14400363385408499</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
+      <c r="B124">
+        <v>0.27633162665192001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
+      <c r="B125">
+        <v>0.26040649711906499</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
+      <c r="B126">
+        <v>0.24433172450489399</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+      <c r="B127">
+        <v>1.8277819846912799</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
+      <c r="B128">
+        <v>0.27806906687794902</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
+      <c r="B129">
+        <v>0.177974625635927</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
+      <c r="B130">
+        <v>0.198879466263954</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
+      <c r="B131">
+        <v>0.27749395630172702</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
+      <c r="B132">
+        <v>0.14400363385408499</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
+      <c r="B133">
+        <v>0.181315298915499</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
+      <c r="B134">
+        <v>0.25165529514783702</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
+      <c r="B135">
+        <v>0.17635543188865499</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
+      <c r="B136">
+        <v>0.80060083208168697</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
+      <c r="B137">
+        <v>0.33333336828892202</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
+      <c r="B138">
+        <v>0.23280492448915099</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
+      <c r="B139">
+        <v>1.44240203460497</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
+      <c r="B140">
+        <v>0.29128398340571898</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
+      <c r="B141">
+        <v>0.28842646242172698</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
+      <c r="B142">
+        <v>0.34339566367742302</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
+      <c r="B143">
+        <v>0.26756915543682402</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
+      <c r="B144">
+        <v>0.28200089518535199</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
+      <c r="B145">
+        <v>0.18980685106235501</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
+      <c r="B146">
+        <v>0.50698862759057195</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
+      <c r="B147">
+        <v>0.13998273091512101</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
+      <c r="B148">
+        <v>0.33564258761597099</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
+      <c r="B149">
+        <v>0.24745170879134801</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
+      <c r="B150">
+        <v>0.60959492638014001</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
+      <c r="B151">
+        <v>0.288730503429796</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
+      <c r="B152">
+        <v>0.31435362346896401</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
+      <c r="B153">
+        <v>0.21251988038596101</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
+      <c r="B154">
+        <v>0.22173757076676101</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
+      <c r="B155">
+        <v>0.38076151403782998</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
+      <c r="B156">
+        <v>0.33333335780224499</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
+      <c r="B157">
+        <v>0.15139547554886401</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A157" t="s">
+      <c r="B158">
+        <v>0.33333335780224499</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
+      <c r="B159">
+        <v>1.24817583475813</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
+      <c r="B160">
+        <v>0.258804491121439</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
+      <c r="B161">
+        <v>0.22154405626281901</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
+      <c r="B162">
+        <v>0.17063633876852399</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
+      <c r="B163">
+        <v>0.22266512546428699</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
+      <c r="B164">
+        <v>0.26826678095317202</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
+      <c r="B165">
+        <v>0.25217122405356801</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
+      <c r="B166">
+        <v>0.70865384981229196</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A166" t="s">
+      <c r="B167">
+        <v>0.24888021063193799</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
+      <c r="B168">
+        <v>0.62679184132184196</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A168" t="s">
+      <c r="B169">
+        <v>0.14400363385408499</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
+      <c r="B170">
+        <v>0.41012890844778199</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A170" t="s">
+      <c r="B171">
+        <v>0.34538874301169897</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
+      <c r="B172">
+        <v>0.13481660083529201</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A172" t="s">
+      <c r="B173">
+        <v>0.25709037218171699</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A173" t="s">
+      <c r="B174">
+        <v>0.28373100894891001</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
         <v>350</v>
+      </c>
+      <c r="B175">
+        <v>0.14400363385408499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add information of average degree
</commit_message>
<xml_diff>
--- a/ComplexNetwork1/src/result/CA.xlsx
+++ b/ComplexNetwork1/src/result/CA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="connected component" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="352">
   <si>
     <t>[CAYWK]</t>
   </si>
@@ -1078,6 +1078,9 @@
   </si>
   <si>
     <t>CAYZP</t>
+  </si>
+  <si>
+    <t>the average degree</t>
   </si>
 </sst>
 </file>
@@ -1423,40 +1426,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B8">
+        <v>4.3023255813953396</v>
       </c>
     </row>
   </sheetData>
@@ -7105,7 +7117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{316DB294-BC15-4EE8-975C-59A65540C50A}">
   <dimension ref="A1:B175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>